<commit_message>
Página de login feita
</commit_message>
<xml_diff>
--- a/Documentos/Backlog/Orgulho Alvinegro - Product Backlog.xlsx
+++ b/Documentos/Backlog/Orgulho Alvinegro - Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/lucas_santos114_sptech_school/Documents/DEV/SPTECH/1SEMESTRE(JANEIRO 2024 - JUNHO 2024)/sprint3/PESQUISAEINOVAÇÃO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documentos\projeto de pi\Orgulho-Alvinegro\Documentos\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="294" documentId="8_{E5571C23-6D6D-4B95-B21E-ED95307A9832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64855D65-AE20-4371-AC4C-D43105EB5AA9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0964C980-CBAA-4C0D-8D0A-AC96A14573CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -608,9 +608,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -675,6 +672,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,6 +719,36 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -787,52 +817,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -852,6 +836,22 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -911,12 +911,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="C6:H37" headerRowDxfId="6" totalsRowDxfId="7" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="C6:H37" headerRowDxfId="7" totalsRowDxfId="6" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="C6:H37" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requisitos" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descrição" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Classificação" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requisitos" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descrição" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Classificação" dataDxfId="3" dataCellStyle="Normal"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Tamanho" dataDxfId="2" dataCellStyle="Normal"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Tam (#)" dataDxfId="1" dataCellStyle="Normal"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Prioridade" dataDxfId="0" dataCellStyle="Normal"/>
@@ -1125,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E13" sqref="E12:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1153,725 +1153,725 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="2:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="2:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>8</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="2:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>5</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>5</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="2:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>8</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="2:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>13</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="5"/>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="2:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>85</v>
       </c>
       <c r="E12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="5">
+        <v>3</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="2:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="5">
+        <v>5</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="2:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F14" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="2:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="5">
+        <v>8</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F16" s="5">
+        <v>21</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="5">
+        <v>21</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="5">
+        <v>8</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="5">
+        <v>3</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="5">
+        <v>13</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="5">
+        <v>8</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="5">
+        <v>8</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="5">
+        <v>21</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="5">
+        <v>8</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="5">
+        <v>8</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="5">
+        <v>13</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="5">
+        <v>8</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="5">
+        <v>13</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="5">
+        <v>8</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="5">
+        <v>13</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="5">
         <v>5</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G31" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="2:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="6">
-        <v>3</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="5">
+        <v>21</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="5">
         <v>8</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G33" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="14" t="s">
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F34" s="22">
+        <v>8</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="23"/>
+    </row>
+    <row r="35" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="24">
+        <v>13</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="24">
         <v>21</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="14" t="s">
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="6">
-        <v>21</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="6">
+      <c r="F37" s="24">
+        <v>13</v>
+      </c>
+      <c r="G37" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="6">
-        <v>3</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="2:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="6">
-        <v>13</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="6">
-        <v>8</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="6">
-        <v>8</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="6">
-        <v>21</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="6">
-        <v>8</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F25" s="6">
-        <v>8</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="6">
-        <v>13</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="6">
-        <v>8</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="6">
-        <v>13</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="6">
-        <v>8</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F30" s="6">
-        <v>13</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" s="6">
-        <v>5</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="6">
-        <v>21</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="6">
-        <v>8</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33" s="6"/>
-    </row>
-    <row r="34" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="23">
-        <v>8</v>
-      </c>
-      <c r="G34" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H34" s="24"/>
-    </row>
-    <row r="35" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="25">
-        <v>13</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="25">
-        <v>21</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="8"/>
-    </row>
-    <row r="37" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="25">
-        <v>13</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37" s="8"/>
+      <c r="H37" s="7"/>
     </row>
     <row r="38" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
     </row>
     <row r="39" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
     </row>
     <row r="40" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>

</xml_diff>

<commit_message>
Mensagem no login e bug arrumado
</commit_message>
<xml_diff>
--- a/Documentos/Backlog/Orgulho Alvinegro - Product Backlog.xlsx
+++ b/Documentos/Backlog/Orgulho Alvinegro - Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documentos\projetopi\Orgulho-Alvinegro\Documentos\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D296BE7-A001-487A-9229-27875ADDD0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD114F0-8007-426A-BF5C-04ABACFBD963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="115">
   <si>
     <t>PRODUCT BACKLOG - PHOENIX EYE (GRUPO 2)</t>
   </si>
@@ -358,17 +358,42 @@
   </si>
   <si>
     <t>Desenvolvimento da página Camisas.Nela terá uma diversidade de camisas do clube</t>
+  </si>
+  <si>
+    <t>Comentários em página título</t>
+  </si>
+  <si>
+    <t>Comentários na página título com data do comentário e imagem do usuário.</t>
+  </si>
+  <si>
+    <t>Comentários em página ídolos</t>
+  </si>
+  <si>
+    <t>Comentários na página ídolo com data do comentário e imagem do usuário.</t>
+  </si>
+  <si>
+    <t>Adição de foto no cadastro</t>
+  </si>
+  <si>
+    <t>O usuário poderá adicionar uma foto ao seu perfil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -479,7 +504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -594,37 +619,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -633,22 +664,25 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -657,12 +691,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1096,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1286,118 +1346,118 @@
     </row>
     <row r="12" spans="2:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>7</v>
+        <v>113</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="F12" s="5">
-        <v>3</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>8</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>84</v>
+        <v>46</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>76</v>
+        <v>84</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="F14" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>77</v>
+        <v>86</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="F15" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>7</v>
+        <v>49</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="F16" s="5">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>89</v>
+        <v>50</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>7</v>
@@ -1412,97 +1472,97 @@
     </row>
     <row r="18" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="5">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>76</v>
+        <v>90</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="F19" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="2:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>7</v>
+        <v>91</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="F20" s="5">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="30">
+        <v>13</v>
+      </c>
+      <c r="G21" s="21" t="s">
         <v>8</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>7</v>
@@ -1517,55 +1577,55 @@
     </row>
     <row r="23" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="5">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>96</v>
+        <v>31</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>77</v>
+        <v>95</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="F24" s="5">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>77</v>
@@ -1580,37 +1640,37 @@
     </row>
     <row r="26" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>58</v>
+        <v>33</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>7</v>
+        <v>98</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="F26" s="5">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>59</v>
+        <v>32</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>109</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>7</v>
+        <v>110</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="F27" s="5">
         <v>8</v>
@@ -1622,166 +1682,166 @@
     </row>
     <row r="28" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>60</v>
+        <v>33</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>7</v>
+        <v>112</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="F28" s="5">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F29" s="5">
+        <v>13</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>72</v>
+        <v>35</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>77</v>
+        <v>101</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="F30" s="5">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F31" s="5">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="H31" s="4"/>
     </row>
     <row r="32" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F32" s="5">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>79</v>
+        <v>38</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>7</v>
+        <v>102</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="F33" s="5">
+        <v>13</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>106</v>
+        <v>39</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="19">
-        <v>8</v>
-      </c>
-      <c r="G34" s="21" t="s">
-        <v>9</v>
+      <c r="F34" s="5">
+        <v>5</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>20</v>
+        <v>80</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>104</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="20">
-        <v>13</v>
+      <c r="F35" s="5">
+        <v>21</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>14</v>
@@ -1790,157 +1850,255 @@
     </row>
     <row r="36" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>107</v>
+        <v>79</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>105</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="20">
-        <v>21</v>
+      <c r="F36" s="5">
+        <v>8</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>22</v>
+        <v>75</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="20">
+      <c r="F37" s="19">
+        <v>8</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="20">
         <v>13</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="26"/>
+    </row>
+    <row r="39" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="20">
+        <v>21</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="26"/>
+    </row>
+    <row r="40" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="19">
+        <v>13</v>
+      </c>
+      <c r="G40" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="1"/>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="1"/>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="1"/>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="1"/>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="1"/>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="1"/>
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="1"/>
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="1"/>
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="1"/>
-      <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="1"/>
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="1"/>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="1"/>
-      <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="1"/>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="1"/>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="1"/>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="1"/>
-      <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H40" s="26"/>
+    </row>
+    <row r="41" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="32"/>
+    </row>
+    <row r="42" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+    </row>
+    <row r="45" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+    </row>
+    <row r="46" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+    </row>
+    <row r="47" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+    </row>
+    <row r="48" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+    </row>
+    <row r="49" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+    </row>
+    <row r="50" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+    </row>
+    <row r="51" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+    </row>
+    <row r="52" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+    </row>
+    <row r="53" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+    </row>
+    <row r="54" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+    </row>
+    <row r="55" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+    </row>
+    <row r="56" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D56" s="1"/>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D57" s="1"/>
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D58" s="1"/>
       <c r="E58" s="2"/>
     </row>
-    <row r="59" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D59" s="1"/>
       <c r="E59" s="2"/>
     </row>
-    <row r="60" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D60" s="1"/>
       <c r="E60" s="2"/>
     </row>
-    <row r="61" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D61" s="1"/>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D62" s="1"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D63" s="1"/>
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D64" s="1"/>
       <c r="E64" s="2"/>
     </row>
@@ -5700,7 +5858,7 @@
   <mergeCells count="1">
     <mergeCell ref="B3:H4"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>